<commit_message>
Revert "excel file v4"
This reverts commit f363d55995a8b449f674a42292b7a3d069651034.
</commit_message>
<xml_diff>
--- a/Telia/TeliaMVC/Content/ExcelFile.xlsx
+++ b/Telia/TeliaMVC/Content/ExcelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jovan\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0B1B91-3475-48BF-9D08-793A7AB6AEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A712EC-C3F2-42DF-8672-6E567AB525D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{6186F350-2FE8-466B-B875-DABA5603F9DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{5FB896A6-100B-4DC6-A5AC-6FCBE45D88C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Telefonnummer</t>
   </si>
@@ -84,40 +84,34 @@
     <t>Kostnadsted</t>
   </si>
   <si>
-    <t>Dobbel Fri</t>
-  </si>
-  <si>
-    <t>Jovan</t>
-  </si>
-  <si>
-    <t>Miladinovic</t>
-  </si>
-  <si>
-    <t>Pristina</t>
-  </si>
-  <si>
-    <t>jovanmczv1@gmail.com</t>
-  </si>
-  <si>
-    <t>Jovanmczv1@gmail.com</t>
+    <t>Adresaa</t>
+  </si>
+  <si>
+    <t>Adresa</t>
+  </si>
+  <si>
+    <t>1@1</t>
   </si>
   <si>
     <t>Faktura 1</t>
   </si>
   <si>
-    <t>Dobbel 6 GB</t>
-  </si>
-  <si>
-    <t>Marko</t>
-  </si>
-  <si>
-    <t>Miloradovic</t>
-  </si>
-  <si>
-    <t>Negotin</t>
-  </si>
-  <si>
-    <t>marko.miloradovic@elfak.rs</t>
+    <t>2@2</t>
+  </si>
+  <si>
+    <t>Faktura 2</t>
+  </si>
+  <si>
+    <t>3@3</t>
+  </si>
+  <si>
+    <t>Faktura 3</t>
+  </si>
+  <si>
+    <t>Dobbel 15 GB</t>
+  </si>
+  <si>
+    <t>EHF</t>
   </si>
 </sst>
 </file>
@@ -501,11 +495,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7333DC-B38E-4747-B536-183D58B4FE64}">
-  <dimension ref="A1:Q3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AE70A9-A8AD-4B50-B706-37C621761B97}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,127 +569,179 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>47589754</v>
+        <v>484848484</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>121</v>
-      </c>
-      <c r="J2">
-        <v>11</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="M2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="N2">
         <v>5</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>97541827</v>
+        <v>487897214</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>122</v>
-      </c>
       <c r="J3">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="N3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P3">
         <v>2</v>
       </c>
       <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>48487897</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{5211FE97-9DFB-4643-AA04-8F9D338A06B7}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{6F70F635-4116-4F59-BC6B-A5BBCED6D7DF}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{F41AAB08-D4FB-41C7-8339-E94238EEB7CB}"/>
-    <hyperlink ref="M3" r:id="rId4" xr:uid="{15A4C90E-125C-4EEA-B33D-3292FB442F02}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{3E082815-7F20-4A66-9AAD-F7B1BEE6B1DF}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{8EC0EF07-2D67-4527-8B84-225EDC75D209}"/>
+    <hyperlink ref="L3" r:id="rId3" xr:uid="{866A4BB2-AA3F-40D0-BEAC-E2D144056D76}"/>
+    <hyperlink ref="M3" r:id="rId4" xr:uid="{A9981764-F0CB-4611-AA34-9C8CC3586AAE}"/>
+    <hyperlink ref="L4" r:id="rId5" xr:uid="{0D2A7E27-2D26-4497-A500-E2BA83D5DA1F}"/>
+    <hyperlink ref="M4" r:id="rId6" xr:uid="{13E821FB-8FE2-4BED-8150-0706AE9265FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>